<commit_message>
Aset Sarana Fixed Table
</commit_message>
<xml_diff>
--- a/project/aset/01. PENERIMAAN DAN PENDISTRIBUSIAN BARANG.xlsx
+++ b/project/aset/01. PENERIMAAN DAN PENDISTRIBUSIAN BARANG.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27126"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Larashit\ermsimrsmu\project\aset\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22A5AF7F-FA76-4DA5-892D-FBEC570C1A17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0959F31-B035-41A6-B437-75107CC67A62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2021" sheetId="1" r:id="rId1"/>
@@ -4397,10 +4397,22 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -4417,18 +4429,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -47660,7 +47660,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A2:N271"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A100" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="R257" sqref="R257"/>
     </sheetView>
   </sheetViews>
@@ -47671,7 +47671,7 @@
     <col min="3" max="3" width="23.85546875" customWidth="1"/>
     <col min="4" max="4" width="22.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="17.7109375" style="5" customWidth="1"/>
-    <col min="6" max="7" width="18" style="162" customWidth="1"/>
+    <col min="6" max="7" width="30.7109375" style="162" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="15.85546875" customWidth="1"/>
     <col min="9" max="9" width="18" customWidth="1"/>
     <col min="10" max="10" width="17.7109375" customWidth="1"/>
@@ -57185,9 +57185,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:N219"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A74" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="Q6" sqref="Q6"/>
+      <selection pane="bottomLeft" activeCell="P87" sqref="P87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -58186,7 +58186,7 @@
       </c>
     </row>
     <row r="31" spans="1:13" s="181" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="239" t="s">
+      <c r="A31" s="243" t="s">
         <v>862</v>
       </c>
       <c r="B31" s="20" t="s">
@@ -58215,7 +58215,7 @@
       </c>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A32" s="239"/>
+      <c r="A32" s="243"/>
       <c r="B32" s="20" t="s">
         <v>905</v>
       </c>
@@ -58242,7 +58242,7 @@
       </c>
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A33" s="239"/>
+      <c r="A33" s="243"/>
       <c r="B33" s="20" t="s">
         <v>906</v>
       </c>
@@ -58269,7 +58269,7 @@
       </c>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A34" s="239"/>
+      <c r="A34" s="243"/>
       <c r="B34" s="20" t="s">
         <v>907</v>
       </c>
@@ -58296,7 +58296,7 @@
       </c>
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A35" s="239"/>
+      <c r="A35" s="243"/>
       <c r="B35" s="20" t="s">
         <v>908</v>
       </c>
@@ -59214,13 +59214,13 @@
       </c>
     </row>
     <row r="61" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A61" s="240"/>
-      <c r="B61" s="241"/>
-      <c r="C61" s="241"/>
-      <c r="D61" s="241"/>
-      <c r="E61" s="241"/>
-      <c r="F61" s="241"/>
-      <c r="G61" s="242"/>
+      <c r="A61" s="244"/>
+      <c r="B61" s="245"/>
+      <c r="C61" s="245"/>
+      <c r="D61" s="245"/>
+      <c r="E61" s="245"/>
+      <c r="F61" s="245"/>
+      <c r="G61" s="246"/>
       <c r="H61" s="2" t="s">
         <v>972</v>
       </c>
@@ -59728,10 +59728,10 @@
       </c>
     </row>
     <row r="77" spans="1:13" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A77" s="239" t="s">
+      <c r="A77" s="243" t="s">
         <v>991</v>
       </c>
-      <c r="B77" s="243" t="s">
+      <c r="B77" s="247" t="s">
         <v>992</v>
       </c>
       <c r="C77" s="20" t="s">
@@ -59761,8 +59761,8 @@
       </c>
     </row>
     <row r="78" spans="1:13" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A78" s="239"/>
-      <c r="B78" s="243"/>
+      <c r="A78" s="243"/>
+      <c r="B78" s="247"/>
       <c r="C78" s="20" t="s">
         <v>869</v>
       </c>
@@ -59868,7 +59868,7 @@
       <c r="B81" s="2" t="s">
         <v>998</v>
       </c>
-      <c r="C81" s="237" t="s">
+      <c r="C81" s="242" t="s">
         <v>869</v>
       </c>
       <c r="D81" s="238">
@@ -59891,7 +59891,7 @@
       <c r="B82" s="3" t="s">
         <v>999</v>
       </c>
-      <c r="C82" s="237"/>
+      <c r="C82" s="242"/>
       <c r="D82" s="238"/>
       <c r="E82" s="161">
         <v>45118</v>
@@ -59918,7 +59918,7 @@
       <c r="B83" s="3" t="s">
         <v>1000</v>
       </c>
-      <c r="C83" s="237"/>
+      <c r="C83" s="242"/>
       <c r="D83" s="238"/>
       <c r="E83" s="161">
         <v>45118</v>
@@ -59945,7 +59945,7 @@
       <c r="B84" s="3" t="s">
         <v>1001</v>
       </c>
-      <c r="C84" s="237"/>
+      <c r="C84" s="242"/>
       <c r="D84" s="238"/>
       <c r="E84" s="161">
         <v>45118</v>
@@ -59972,7 +59972,7 @@
       <c r="B85" s="3" t="s">
         <v>1002</v>
       </c>
-      <c r="C85" s="237"/>
+      <c r="C85" s="242"/>
       <c r="D85" s="238"/>
       <c r="E85" s="161">
         <v>45118</v>
@@ -59999,7 +59999,7 @@
       <c r="B86" s="3" t="s">
         <v>1003</v>
       </c>
-      <c r="C86" s="237"/>
+      <c r="C86" s="242"/>
       <c r="D86" s="238"/>
       <c r="E86" s="161">
         <v>45118</v>
@@ -60026,7 +60026,7 @@
       <c r="B87" s="3" t="s">
         <v>1004</v>
       </c>
-      <c r="C87" s="237"/>
+      <c r="C87" s="242"/>
       <c r="D87" s="238"/>
       <c r="E87" s="161">
         <v>45118</v>
@@ -60053,7 +60053,7 @@
       <c r="B88" s="3" t="s">
         <v>1005</v>
       </c>
-      <c r="C88" s="237"/>
+      <c r="C88" s="242"/>
       <c r="D88" s="238"/>
       <c r="E88" s="161">
         <v>45118</v>
@@ -60080,7 +60080,7 @@
       <c r="B89" s="3" t="s">
         <v>1006</v>
       </c>
-      <c r="C89" s="237"/>
+      <c r="C89" s="242"/>
       <c r="D89" s="238"/>
       <c r="E89" s="161">
         <v>45118</v>
@@ -60107,7 +60107,7 @@
       <c r="B90" s="3" t="s">
         <v>1010</v>
       </c>
-      <c r="C90" s="237"/>
+      <c r="C90" s="242"/>
       <c r="D90" s="238"/>
       <c r="E90" s="161">
         <v>45118</v>
@@ -62150,7 +62150,7 @@
       <c r="C147" s="201" t="s">
         <v>875</v>
       </c>
-      <c r="D147" s="245">
+      <c r="D147" s="239">
         <v>35000000</v>
       </c>
       <c r="E147" s="203">
@@ -62189,7 +62189,7 @@
       <c r="C148" s="201" t="s">
         <v>875</v>
       </c>
-      <c r="D148" s="247"/>
+      <c r="D148" s="241"/>
       <c r="E148" s="203">
         <v>45177</v>
       </c>
@@ -62694,7 +62694,7 @@
       <c r="C161" s="2" t="s">
         <v>869</v>
       </c>
-      <c r="D161" s="245">
+      <c r="D161" s="239">
         <v>23435000</v>
       </c>
       <c r="E161" s="161">
@@ -62733,7 +62733,7 @@
       <c r="C162" s="2" t="s">
         <v>869</v>
       </c>
-      <c r="D162" s="246"/>
+      <c r="D162" s="240"/>
       <c r="E162" s="161">
         <v>45188</v>
       </c>
@@ -62770,7 +62770,7 @@
       <c r="C163" s="2" t="s">
         <v>869</v>
       </c>
-      <c r="D163" s="246"/>
+      <c r="D163" s="240"/>
       <c r="E163" s="161">
         <v>45188</v>
       </c>
@@ -62807,7 +62807,7 @@
       <c r="C164" s="2" t="s">
         <v>869</v>
       </c>
-      <c r="D164" s="247"/>
+      <c r="D164" s="241"/>
       <c r="E164" s="161">
         <v>45188</v>
       </c>
@@ -62844,7 +62844,7 @@
       <c r="C165" s="2" t="s">
         <v>869</v>
       </c>
-      <c r="D165" s="245">
+      <c r="D165" s="239">
         <v>1320000</v>
       </c>
       <c r="E165" s="161">
@@ -62877,7 +62877,7 @@
       <c r="C166" s="2" t="s">
         <v>869</v>
       </c>
-      <c r="D166" s="247"/>
+      <c r="D166" s="241"/>
       <c r="E166" s="161">
         <v>45192</v>
       </c>
@@ -63632,7 +63632,7 @@
       <c r="C189" s="2" t="s">
         <v>869</v>
       </c>
-      <c r="D189" s="244">
+      <c r="D189" s="237">
         <v>3150000</v>
       </c>
       <c r="E189" s="161">
@@ -63671,7 +63671,7 @@
       <c r="C190" s="2" t="s">
         <v>869</v>
       </c>
-      <c r="D190" s="244"/>
+      <c r="D190" s="237"/>
       <c r="E190" s="161">
         <v>45239</v>
       </c>
@@ -64757,11 +64757,6 @@
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="D189:D190"/>
-    <mergeCell ref="D186:D187"/>
-    <mergeCell ref="D161:D164"/>
-    <mergeCell ref="D165:D166"/>
-    <mergeCell ref="D147:D148"/>
     <mergeCell ref="C81:C90"/>
     <mergeCell ref="D81:D90"/>
     <mergeCell ref="D4:D6"/>
@@ -64769,6 +64764,11 @@
     <mergeCell ref="A61:G61"/>
     <mergeCell ref="B77:B78"/>
     <mergeCell ref="A77:A78"/>
+    <mergeCell ref="D189:D190"/>
+    <mergeCell ref="D186:D187"/>
+    <mergeCell ref="D161:D164"/>
+    <mergeCell ref="D165:D166"/>
+    <mergeCell ref="D147:D148"/>
   </mergeCells>
   <pageMargins left="0.13" right="0.12" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="119" scale="90" orientation="landscape" r:id="rId1"/>
@@ -66156,7 +66156,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A2:L46"/>
   <sheetViews>
-    <sheetView topLeftCell="C28" workbookViewId="0">
+    <sheetView topLeftCell="C1" workbookViewId="0">
       <selection activeCell="L4" sqref="L4"/>
     </sheetView>
   </sheetViews>

</xml_diff>